<commit_message>
Add missing algorithm entry to the TSP experiment
</commit_message>
<xml_diff>
--- a/tsp_custom_results.xlsx
+++ b/tsp_custom_results.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10402"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nunofernandes/Desktop/Engenharia informática /EI 2ºANO 2ºSEMESTRE/Inteligência Artificial/DEV/Artificial Intelligence/Prática/TSP - iCidades-1/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7273FA-738C-1D4F-A592-9C784B35A6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="eil51.tsp" sheetId="1" r:id="rId1"/>
     <sheet name="berlin52.tsp" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="11">
   <si>
     <t>Algorithm</t>
   </si>
@@ -52,12 +46,15 @@
   <si>
     <t>rGreedy</t>
   </si>
+  <si>
+    <t>optDistCircularIC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,21 +117,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -172,7 +161,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -206,7 +195,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -241,10 +229,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -417,22 +404,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="55" customWidth="1"/>
-    <col min="2" max="2" width="44.1640625" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" customWidth="1"/>
-    <col min="4" max="4" width="35" customWidth="1"/>
-    <col min="5" max="5" width="33.1640625" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -460,19 +439,19 @@
         <v>100</v>
       </c>
       <c r="C2">
-        <v>0.77190294265747073</v>
+        <v>0.7527199268341065</v>
       </c>
       <c r="D2">
-        <v>1613.5991917688241</v>
+        <v>1690.69556594935</v>
       </c>
       <c r="E2">
-        <v>597.34143346783605</v>
+        <v>587.2384758832502</v>
       </c>
       <c r="F2">
-        <v>62.980804866849759</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65.26645673471631</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -480,19 +459,19 @@
         <v>1000</v>
       </c>
       <c r="C3">
-        <v>0.7706941604614258</v>
+        <v>0.7605681657791138</v>
       </c>
       <c r="D3">
-        <v>1626.8843998062421</v>
+        <v>1606.507632883173</v>
       </c>
       <c r="E3">
-        <v>572.92627505950645</v>
+        <v>601.6161825762687</v>
       </c>
       <c r="F3">
-        <v>64.783836200793331</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>62.55130257323721</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -500,19 +479,19 @@
         <v>10000</v>
       </c>
       <c r="C4">
-        <v>0.83264038562774656</v>
+        <v>0.7604927301406861</v>
       </c>
       <c r="D4">
-        <v>1675.4116729656789</v>
+        <v>1656.525734252777</v>
       </c>
       <c r="E4">
-        <v>575.87583851091608</v>
+        <v>582.0750347067585</v>
       </c>
       <c r="F4">
-        <v>65.627800748723033</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>64.86169682300044</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -520,19 +499,19 @@
         <v>100</v>
       </c>
       <c r="C5">
-        <v>0.77340617179870608</v>
+        <v>0.7391364812850952</v>
       </c>
       <c r="D5">
-        <v>1604.832046040877</v>
+        <v>1669.127478383141</v>
       </c>
       <c r="E5">
-        <v>657.71359650315151</v>
+        <v>629.1458541549424</v>
       </c>
       <c r="F5">
-        <v>59.016671051295873</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>62.3069021208382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -540,19 +519,19 @@
         <v>1000</v>
       </c>
       <c r="C6">
-        <v>0.76359279155731197</v>
+        <v>0.7438838243484497</v>
       </c>
       <c r="D6">
-        <v>1603.89802301501</v>
+        <v>1594.671085733298</v>
       </c>
       <c r="E6">
-        <v>639.52252567260382</v>
+        <v>633.4624096481157</v>
       </c>
       <c r="F6">
-        <v>60.126983355810353</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>60.27629676643803</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -560,19 +539,19 @@
         <v>10000</v>
       </c>
       <c r="C7">
-        <v>0.75500130653381348</v>
+        <v>0.7075989246368408</v>
       </c>
       <c r="D7">
-        <v>1665.5631815385259</v>
+        <v>1694.54631786108</v>
       </c>
       <c r="E7">
-        <v>622.48334368145686</v>
+        <v>641.2655363197239</v>
       </c>
       <c r="F7">
-        <v>62.626254555744197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>62.15709599905459</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -580,19 +559,19 @@
         <v>100</v>
       </c>
       <c r="C8">
-        <v>7.4968099594116206E-3</v>
+        <v>0.009421491622924804</v>
       </c>
       <c r="D8">
-        <v>1695.524201597909</v>
+        <v>1647.523712337971</v>
       </c>
       <c r="E8">
-        <v>1089.3598544440231</v>
+        <v>1053.532215927919</v>
       </c>
       <c r="F8">
-        <v>35.750851953786331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>36.05359315691607</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -600,19 +579,19 @@
         <v>1000</v>
       </c>
       <c r="C9">
-        <v>5.9365034103393546E-3</v>
+        <v>0.006155323982238769</v>
       </c>
       <c r="D9">
-        <v>1677.3765184498741</v>
+        <v>1707.036973975203</v>
       </c>
       <c r="E9">
-        <v>1132.2933404940361</v>
+        <v>1059.096032680611</v>
       </c>
       <c r="F9">
-        <v>32.496173158520747</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37.95705372366496</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -620,19 +599,19 @@
         <v>10000</v>
       </c>
       <c r="C10">
-        <v>6.6450119018554689E-3</v>
+        <v>0.005618906021118164</v>
       </c>
       <c r="D10">
-        <v>1660.261648780315</v>
+        <v>1632.820212375709</v>
       </c>
       <c r="E10">
-        <v>1111.6426281154979</v>
+        <v>1146.085119127346</v>
       </c>
       <c r="F10">
-        <v>33.04413018682034</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>29.80947256527263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -640,19 +619,19 @@
         <v>100</v>
       </c>
       <c r="C11">
-        <v>8.0381570100784305</v>
+        <v>7.845069527626038</v>
       </c>
       <c r="D11">
-        <v>1638.3179544993179</v>
+        <v>1599.786781328893</v>
       </c>
       <c r="E11">
-        <v>572.56871808261803</v>
+        <v>564.2070818171729</v>
       </c>
       <c r="F11">
-        <v>65.051428722356931</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>64.73235756151806</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -660,19 +639,19 @@
         <v>1000</v>
       </c>
       <c r="C12">
-        <v>7.7667384624481199</v>
+        <v>7.759456515312195</v>
       </c>
       <c r="D12">
-        <v>1631.641619599146</v>
+        <v>1680.909565873136</v>
       </c>
       <c r="E12">
-        <v>570.51970118254371</v>
+        <v>578.7020480937815</v>
       </c>
       <c r="F12">
-        <v>65.034006590080338</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65.57208907350235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -680,16 +659,76 @@
         <v>10000</v>
       </c>
       <c r="C13">
-        <v>8.0636532306671143</v>
+        <v>7.626270771026611</v>
       </c>
       <c r="D13">
-        <v>1663.2795353273709</v>
+        <v>1695.828535289568</v>
       </c>
       <c r="E13">
-        <v>568.81433684817057</v>
+        <v>570.2023307639324</v>
       </c>
       <c r="F13">
-        <v>65.801639185308971</v>
+        <v>66.376180203468</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>0.002634811401367188</v>
+      </c>
+      <c r="D14">
+        <v>1697.38957176831</v>
+      </c>
+      <c r="E14">
+        <v>1197.669716218704</v>
+      </c>
+      <c r="F14">
+        <v>29.44049285215102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>1000</v>
+      </c>
+      <c r="C15">
+        <v>0.02549126148223877</v>
+      </c>
+      <c r="D15">
+        <v>1671.500762575172</v>
+      </c>
+      <c r="E15">
+        <v>761.8136826246156</v>
+      </c>
+      <c r="F15">
+        <v>54.4233721167474</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>10000</v>
+      </c>
+      <c r="C16">
+        <v>0.2539310455322266</v>
+      </c>
+      <c r="D16">
+        <v>1640.326677750452</v>
+      </c>
+      <c r="E16">
+        <v>569.2512753969586</v>
+      </c>
+      <c r="F16">
+        <v>65.29646910470106</v>
       </c>
     </row>
   </sheetData>
@@ -698,14 +737,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -725,7 +764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -733,19 +772,19 @@
         <v>100</v>
       </c>
       <c r="C2">
-        <v>0.94106047153472905</v>
+        <v>0.8538057327270507</v>
       </c>
       <c r="D2">
-        <v>29807.506066294529</v>
+        <v>30152.46355144759</v>
       </c>
       <c r="E2">
-        <v>10022.827129609759</v>
+        <v>10562.62370460025</v>
       </c>
       <c r="F2">
-        <v>66.374821471752441</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>64.96928456085256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -753,19 +792,19 @@
         <v>1000</v>
       </c>
       <c r="C3">
-        <v>0.95051848888397217</v>
+        <v>0.9253467798233033</v>
       </c>
       <c r="D3">
-        <v>29874.704772433812</v>
+        <v>30137.48415372318</v>
       </c>
       <c r="E3">
-        <v>10241.080248821791</v>
+        <v>10476.30416239182</v>
       </c>
       <c r="F3">
-        <v>65.719894717515288</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65.23829225772457</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -773,19 +812,19 @@
         <v>10000</v>
       </c>
       <c r="C4">
-        <v>0.79425725936889646</v>
+        <v>0.8165324926376343</v>
       </c>
       <c r="D4">
-        <v>30633.717984282459</v>
+        <v>30539.66940284299</v>
       </c>
       <c r="E4">
-        <v>10452.43140670003</v>
+        <v>10398.78358613187</v>
       </c>
       <c r="F4">
-        <v>65.879324827423957</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65.94991435904728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -793,19 +832,19 @@
         <v>100</v>
       </c>
       <c r="C5">
-        <v>0.93344781398773191</v>
+        <v>0.9262724637985229</v>
       </c>
       <c r="D5">
-        <v>28952.01423316792</v>
+        <v>30507.73393482665</v>
       </c>
       <c r="E5">
-        <v>10824.43875155826</v>
+        <v>10805.075173917</v>
       </c>
       <c r="F5">
-        <v>62.612484698361357</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>64.58250489203895</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -813,19 +852,19 @@
         <v>1000</v>
       </c>
       <c r="C6">
-        <v>0.94888122081756587</v>
+        <v>0.911911416053772</v>
       </c>
       <c r="D6">
-        <v>30319.574506565801</v>
+        <v>30277.26512266933</v>
       </c>
       <c r="E6">
-        <v>11473.250081911659</v>
+        <v>11100.15033344575</v>
       </c>
       <c r="F6">
-        <v>62.158934389309792</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>63.3383322817529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -833,19 +872,19 @@
         <v>10000</v>
       </c>
       <c r="C7">
-        <v>0.92993927001953125</v>
+        <v>0.90787672996521</v>
       </c>
       <c r="D7">
-        <v>29684.242223618701</v>
+        <v>29982.78027562029</v>
       </c>
       <c r="E7">
-        <v>10843.004798442091</v>
+        <v>10917.22045157333</v>
       </c>
       <c r="F7">
-        <v>63.472185960621587</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>63.58836521758331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -853,19 +892,19 @@
         <v>100</v>
       </c>
       <c r="C8">
-        <v>6.1429023742675783E-3</v>
+        <v>0.005371356010437011</v>
       </c>
       <c r="D8">
-        <v>30609.2573202042</v>
+        <v>29682.95006901009</v>
       </c>
       <c r="E8">
-        <v>20297.87233866828</v>
+        <v>20363.96588755763</v>
       </c>
       <c r="F8">
-        <v>33.687145276568657</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31.39507414117091</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -873,19 +912,19 @@
         <v>1000</v>
       </c>
       <c r="C9">
-        <v>5.1850795745849608E-3</v>
+        <v>0.004100418090820313</v>
       </c>
       <c r="D9">
-        <v>29739.47864426512</v>
+        <v>29632.53728529375</v>
       </c>
       <c r="E9">
-        <v>20230.535672951199</v>
+        <v>21742.72220438267</v>
       </c>
       <c r="F9">
-        <v>31.974141460437469</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26.62551304652099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -893,19 +932,19 @@
         <v>10000</v>
       </c>
       <c r="C10">
-        <v>5.7384490966796873E-3</v>
+        <v>0.008357238769531251</v>
       </c>
       <c r="D10">
-        <v>29578.024535847278</v>
+        <v>29863.53053316114</v>
       </c>
       <c r="E10">
-        <v>20110.777225228849</v>
+        <v>18516.14271628337</v>
       </c>
       <c r="F10">
-        <v>32.007706596985663</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37.99747589883042</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -913,19 +952,19 @@
         <v>100</v>
       </c>
       <c r="C11">
-        <v>9.4928064107894894</v>
+        <v>9.090412235260009</v>
       </c>
       <c r="D11">
-        <v>30984.122632400591</v>
+        <v>29580.71606880549</v>
       </c>
       <c r="E11">
-        <v>10084.10494068419</v>
+        <v>10127.51129329761</v>
       </c>
       <c r="F11">
-        <v>67.453960015833786</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>65.76313004140684</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -933,19 +972,19 @@
         <v>1000</v>
       </c>
       <c r="C12">
-        <v>9.570740890502929</v>
+        <v>9.186949181556702</v>
       </c>
       <c r="D12">
-        <v>29789.674823390491</v>
+        <v>30192.33527117213</v>
       </c>
       <c r="E12">
-        <v>10135.12953965727</v>
+        <v>10022.06245095608</v>
       </c>
       <c r="F12">
-        <v>65.977710063154888</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>66.80593812653761</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -953,16 +992,76 @@
         <v>10000</v>
       </c>
       <c r="C13">
-        <v>10.104649496078491</v>
+        <v>9.017185378074647</v>
       </c>
       <c r="D13">
-        <v>30398.962457180289</v>
+        <v>29719.36782169909</v>
       </c>
       <c r="E13">
-        <v>9980.1293726781114</v>
+        <v>10105.0933784091</v>
       </c>
       <c r="F13">
-        <v>67.169506568732288</v>
+        <v>65.99828960348529</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>0.00268561840057373</v>
+      </c>
+      <c r="D14">
+        <v>29781.35333994811</v>
+      </c>
+      <c r="E14">
+        <v>20982.49073317652</v>
+      </c>
+      <c r="F14">
+        <v>29.54487160584799</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>1000</v>
+      </c>
+      <c r="C15">
+        <v>0.02612676620483399</v>
+      </c>
+      <c r="D15">
+        <v>30520.52860017783</v>
+      </c>
+      <c r="E15">
+        <v>13595.46777012297</v>
+      </c>
+      <c r="F15">
+        <v>55.45467790474719</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>10000</v>
+      </c>
+      <c r="C16">
+        <v>0.2601830959320068</v>
+      </c>
+      <c r="D16">
+        <v>28944.99884145063</v>
+      </c>
+      <c r="E16">
+        <v>10457.27042856887</v>
+      </c>
+      <c r="F16">
+        <v>63.87192659481624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>